<commit_message>
added more variables and created USD deflated stock indices
</commit_message>
<xml_diff>
--- a/examples/raw/N225.xlsx
+++ b/examples/raw/N225.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78fea0453942dc16/Programming/AnomDetect/examples/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77FFF952-D8B0-4311-A4A6-96102F9BD386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{77FFF952-D8B0-4311-A4A6-96102F9BD386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{617DC5E2-BC1A-4B0A-848D-CAA2D2C3241B}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1740" windowWidth="21285" windowHeight="11385"/>
+    <workbookView xWindow="3930" yWindow="1800" windowWidth="21285" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N225" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,22 +44,22 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Adj Close</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
     <t>N225</t>
   </si>
+  <si>
+    <t>N225_LND</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -884,11 +894,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,16 +917,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>